<commit_message>
Minor changes in excel sheet
</commit_message>
<xml_diff>
--- a/questions/questions.xlsx
+++ b/questions/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samboyadvance/corona_faq/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6AE895-4EBF-1845-AB21-B116244DB791}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0233B6C9-DF2B-734D-87B8-8C8A84318282}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" activeTab="1" xr2:uid="{A2092434-8E9F-7046-A332-FF9F1643DB7C}"/>
   </bookViews>
@@ -85,9 +85,6 @@
     <t>कोरोना वायरस एक प्रकार का ऐसा वायरस है, जिसके कारण जानवरों या मनुष्यों में सामान्य सर्दी या बहुत तेज बुखार  या कई गंभीर बीमारियां होती हैं । कोविड 19 कोरोना वायरस का ही एक रूप है, जो हालही में 2019 में चीन में प्रकट हुआ है और वहां से यह भारत सहित विश्व के विभिन्न देशों में फैल गया है ।</t>
   </si>
   <si>
-    <t>कोविड 19 के सबसे ज्यादा सामान्य लक्षण बुखार, थकान तथा सूखी खांसी हैं । कुछ रोगियों को शरीर में दर्द, नाक बंद होना, नाक बहना यानि जुकाम, गले में दर्द या दस्त हो सकता है । आरंभ में ये लक्षण ज्यादातर हल्के रूप में सामने आते हैं और धीरे-धीरे बढ़ने लगते हैं । कुछ लोग संक्रमित होते हैं, फिरभी उनमें कोई लक्षण दिखाई नहीं देता है - लेकिन वे स्वयं को अच्छा महसूस भी नहीं करते हैं । अधिकांश लोग (करीब 80%) बिना विशेष उपचार के ही इस रोग से ठीक हो जाते हैं । कोविड 19 से संक्रमित 06 में से लगभग 01व्यक्ति ही गंभीर रूप से बीमार होते हैं और उन्हें सांस लेने में कठिनाई होती है । वृद्ध व्यक्ति तथा वे लोग ही ज्यादा गंभीर रूप से बीमार होते हैं, जिन्हें हाई ब्लड-प्रेशर, हृदय संबंधी बीमारियां या डायबिटीज है । बुखार, कफ तथा सांस लेने में कष्ट होने पर लोगों को मेडिकल उपचार कराना चाहिए ।</t>
-  </si>
-  <si>
     <t>&lt;ul&gt; &lt;li&gt; अपना हाथ साबुन तथा पानी से  या अल्कोहल मिश्रित हैंड सैनिटाइजर से नियमित एवं उचित रूप से अच्छी तरह धोएं और साफ रखें । इससे हाथ में लगे वायरस मर जाते हैं । &lt;/li&gt;
 &lt;li&gt;खांसने या छींकने वाले व्यक्ति से कम-से-कम 1 मीटर या 3 फीट की दूरी हमेशा बनाएं रखें । जब कोई व्यक्ति खांसता या छींकता है तो उसके मुंह या नाक से छोटी-छोटी बूंदें/ छींटें  निकलती हैं, जिनमें वायरस हो सकते हैं । यदि आप ऐसे व्यक्ति के ज्यादा नजदीक रहेंगे तो आपकी सांसों के माध्यम से ये छींटें  भीतर जा सकती हैं और इस तरह यदि खांसने/ छींकने वाला व्यक्ति संक्रमित है तो आप भी कोविड 19 से संक्रमित हो सकते हैं ।&lt;/li&gt;
 &lt;li&gt;आंख, नाक तथा मुंह छूने से बचें । &lt;/li&gt;
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>कोविड 19 से संक्रमित व्यक्तियों के स्पर्श में आने पर लोग इस वायरस से संक्रमित हो सकते हैं । यह रोग एक व्यक्ति से दूसरे व्यक्ति तक नाक या मुंह से निकली छींटों  के माध्यम से फैलता है । कोविड 19 से संक्रमित व्यक्ति के छींकने या खांसने से निकली छींटों  से यह रोग फैलता है, क्योंकि किसी वस्तु या सतह पर पड़ी इन बूंदों के स्पर्श में जब कोई दूसरा व्यक्ति आता है और वह उसी हाथ से अपनी आंख, नाक या मुंह छूता है तो वह  व्यक्ति भी कोविड 19 से संक्रमित हो जाता है । संक्रमित व्यक्ति के छींकने या खांसने के दौरान निकली बूंदें  जब पास के दूसरे व्यक्ति द्वारा सांस लेने के माध्यम से उसके भीतर चली जाएं तो वह भी कोविड 19 से संक्रमित हो सकता है । इसीलिए यह बहुत महत्वपूर्ण और जरूरी है कि बीमार व्यक्ति से कम-से-कम 1 मीटर (3 फीट) से अधिक की दूरी पर रहा जाए ।</t>
+  </si>
+  <si>
+    <t>कोविड 19 के सबसे ज्यादा सामान्य लक्षण बुखार, थकान तथा सूखी खांसी हैं । कुछ रोगियों को शरीर में दर्द, नाक बंद होना, नाक बहना यानि जुकाम, गले में दर्द या दस्त हो सकता है । आरंभ में ये लक्षण ज्यादातर हल्के रूप में सामने आते हैं और धीरे-धीरे बढ़ने लगते हैं । कुछ लोग संक्रमित होते हैं, फिरभी उनमें कोई लक्षण दिखाई नहीं देता है - लेकिन वे स्वयं को अच्छा महसूस भी नहीं करते हैं । अधिकांश लोग (करीब 80%) बिना विशेष उपचार के ही इस रोग से ठीक हो जाते हैं । कोविड 19 से संक्रमित 6 में से लगभग 1व्यक्ति ही गंभीर रूप से बीमार होते हैं और उन्हें सांस लेने में कठिनाई होती है । वृद्ध व्यक्ति तथा वे लोग ही ज्यादा गंभीर रूप से बीमार होते हैं, जिन्हें हाई ब्लड-प्रेशर, हृदय संबंधी बीमारियां या डायबिटीज है । बुखार, कफ तथा सांस लेने में कष्ट होने पर लोगों को मेडिकल उपचार कराना चाहिए ।</t>
   </si>
 </sst>
 </file>
@@ -520,7 +520,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,7 +550,7 @@
         <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -558,7 +558,7 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="119" x14ac:dyDescent="0.2">
@@ -566,7 +566,7 @@
         <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
minor changes in gujarati translation
</commit_message>
<xml_diff>
--- a/questions/questions.xlsx
+++ b/questions/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samboyadvance/corona_faq/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B9BFD0-0054-8945-A086-F820969C3428}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B27FA15-3CB2-3042-BDB4-B8A583156918}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" activeTab="2" xr2:uid="{A2092434-8E9F-7046-A332-FF9F1643DB7C}"/>
   </bookViews>
@@ -115,9 +115,6 @@
     <t>કોરોનાવાયરસ કેવી રીતે ફેલાય છે?</t>
   </si>
   <si>
-    <t>કોવિડ 19 વાયરસ ધરાવતા લોકો પાસેથી બીજા લોકોને વાયરસ પકડી શકે છે. આ રોગ, કોવિડ 19 વાયરસ ધરાવતા રોગી જ્યારે ઉધરસ કરે કે શ્વાસ કાઢે એના નાક અથવા મોંમાંથી નીકળેલા નાના ટીપાં દ્વારા બીજા વ્યક્તિઓમાં આ રોગ ફેલાઈ શકે છે. આ ટીપાં/કણો રોગીના આજુબાજુની વસ્તુઓમાંથી ફેલાઈ જાય છે. જ્યારે બીજા વ્યક્તિઓ આ વસ્તુઓ ને સ્પર્શ કરીને, પછી તેમની આંખો, નાક અથવા મોંને સ્પર્શ કરે ત્યારે કોવિડ 19 પકડી શકે છે. તેથી જ બીમાર વ્યક્તિથી 1 મીટર અથવા 3 ફુટથી વધુ દૂર રહેવું મહત્વપૂર્ણ છે.</t>
-  </si>
-  <si>
     <t>હું કોરોનાવાયરસથી મારી જાતને કેવી રીતે સુરક્ષિત કરી શકું?</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;નિયમિતપણે અને યોગ્ય રીતે તમારા હાથને સાબુ અને પાણીથી ધોવા, અથવા આલ્કોહોલ આધારિત હેન્ડ સેનિટાઇઝરથી સાફ કરવાથી તમારા હાથ પરના વાયરસનો નાશ થાય છે.&lt;/li&gt;&lt;li&gt;કોઈને પણ ખાંસી અથવા છીક આવતી હોય તો એ વ્યક્તિથી 1 મીટર કે 3 ફૂટ ની દોરી બનાવી રાખવી. જ્યારે કોઈને ઉધરસ આવે છે અથવા છીંક આવે છે, ત્યારે તેઓ તેમના નાક અથવા મોંમાંથી નાના ટીપાં છાંટતા હોય છે જેમાં વાયરસ હોઈ શકે છે.&lt;/li&gt;&lt;li&gt;આંખો, નાક અને મોઢાને સ્પર્શ કરવાનું ટાળો.&lt;/li&gt;&lt;li&gt;જ્યારે તમને ઉધરસ આવે કે છીંક આવે ત્યારે તમારા કોણી અથવા રૂમાલથી તમારા મોં અને નાકને ઢાંકવું.&lt;/li&gt;&lt;li&gt;જો તમને અસ્વસ્થ લાગ્યું હોય તો ઘરે રહો. જો તમને તાવ, ઉધરસ અને શ્વાસ લેવામાં તકલીફ હોય, તો તબીબી સહાય મેળવો અને અગાઉથી ફોન કરો.&lt;/li&gt;&lt;li&gt;તમારા સ્થાનિક ક્ષેત્ર આરોગ્ય અધિકારીની સૂચનાઓનું પાલન કરો.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>કોવિડ 19 વાયરસ ધરાવતા લોકો પાસેથી બીજા લોકોને વાયરસ પકડી શકે છે. આ રોગ, કોવિડ 19 વાયરસ ધરાવતા રોગી જ્યારે ઉધરસ કરે કે શ્વાસ કાઢે એના નાક અથવા મોંમાંથી નીકળેલા નાના ટીપાં દ્વારા બીજા વ્યક્તિઓમાં આ રોગ ફેલાઈ શકે છે. આ ટીપાં/કણો રોગીના આજુબાજુની વસ્તુઓમાં ફેલાઈ જાય છે. જ્યારે બીજા વ્યક્તિઓ આ વસ્તુઓ ને સ્પર્શ કરીને, પછી તેમની આંખો, નાક અથવા મોંને સ્પર્શ કરે ત્યારે કોવિડ 19 પકડી શકે છે. તેથી જ બીમાર વ્યક્તિથી 1 મીટર અથવા 3 ફુટથી વધુ દૂર રહેવું મહત્વપૂર્ણ છે.</t>
   </si>
 </sst>
 </file>
@@ -618,7 +618,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,23 +655,23 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
partially added kannada, added malayalam
</commit_message>
<xml_diff>
--- a/questions/questions.xlsx
+++ b/questions/questions.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samboyadvance/corona_faq/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A490CF72-EC61-BB4D-BA11-608080CD74C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A2B30C-3A28-354A-B40E-F5B60F05CA0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" activeTab="3" xr2:uid="{A2092434-8E9F-7046-A332-FF9F1643DB7C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" activeTab="4" xr2:uid="{A2092434-8E9F-7046-A332-FF9F1643DB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
     <sheet name="Hindi" sheetId="2" r:id="rId2"/>
     <sheet name="Gujarati" sheetId="3" r:id="rId3"/>
     <sheet name="Marathi" sheetId="4" r:id="rId4"/>
+    <sheet name="Malayalam" sheetId="5" r:id="rId5"/>
+    <sheet name="Kannada" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>question</t>
   </si>
@@ -160,12 +162,76 @@
   <si>
     <t>कोरोना व्हायरस चे प्रमुख लक्षणं : सुका कोरडा खोकला , ताप आणि थकवा . काही रुग्णांना मधे हे लक्षणं आढळतील : जुलाब , वहाते नाक, बंद नाक किवनहा शरीर वेदना . हि लक्षणं सुरवातीला सौम्य असतील. काही रुग्ण (इन्फेक्टड) म्हणजे संसर्गित होतील पण काहीही लक्षणं आढळणार नाहीत. साधारण पने ५ पैकी १ रुग्ण काहीही विशेष उपचार न घेताच बरे होतात. साधारण पने ६ कोविड १९ रुग्णानं पैकी एक रुग्ण गंभीर आजारी होतो म्हणजेच स्वास घेने अतिशय अवघड होते. वयस्कर व्यकितींना अथवा उच्च रक्तदाब, ह्रदय विकार , मधुमेय (डायबेटीस ) असलेल्या व्यकितींना कोरोना व्हायरस मुळे गंभीर आजार होण्याची शक्यता जास्त असते. ज्या व्यकितींना कोरडा खोकला , ताप आहे अथवा स्वास घेने अवघड वाटतंय त्यांनी डॉक्टरांना भेटावे </t>
   </si>
+  <si>
+    <t>കൊറോണ വൈറസ് / കോവിഡ് 19 എന്താണ്?</t>
+  </si>
+  <si>
+    <t>ജലദോഷം, അല്ലെങ്കിൽ കൂടുതൽ കഠിനമായ രോഗങ്ങൾ എന്നിവ പോലെ മൃഗങ്ങളിലോ മനുഷ്യരിലോ രോഗമുണ്ടാക്കുന്ന ഒരു തരം വൈറസാണ് കൊറോണ വൈറസ്. 2019 ൽ ചൈനയിൽ അടുത്തിടെ കണ്ടെത്തിയ ഒരു തരം കൊറോണ വൈറസാണ് കോവിഡ് 19, ഇത് ഇന്ത്യ ഉൾപ്പെടെ ലോകത്തിന്റെ വിവിധ ഭാഗങ്ങളിലേക്ക് വ്യാപിച്ചു</t>
+  </si>
+  <si>
+    <t>കൊറോണ വൈറസിന്റെ ലക്ഷണങ്ങൾ എന്തൊക്കെയാണ്?</t>
+  </si>
+  <si>
+    <t>പനി, ക്ഷീണം, വരണ്ട ചുമ എന്നിവയാണ് കോവിഡ് 19 ന്റെ ഏറ്റവും സാധാരണമായ ലക്ഷണങ്ങൾ. ചില രോഗികൾക്ക് ശരീരവേദന, മൂക്ക് തടഞ്ഞത്, മൂക്കൊലിപ്പ്, തൊണ്ടവേദന അല്ലെങ്കിൽ വയറിളക്കം എന്നിവ ഉണ്ടാകാം. ഈ ലക്ഷണങ്ങൾ സാധാരണയായി സൗമ്യവും ക്രമേണ ആരംഭിക്കുന്നതുമാണ്. ചില ആളുകൾ രോഗബാധിതരാകുന്നു, പക്ഷേ രോഗലക്ഷണങ്ങളൊന്നും വികസിപ്പിക്കുന്നില്ല, അസുഖം തോന്നുന്നില്ല. 5 പേരിൽ ഒരാൾ പ്രത്യേക ചികിത്സ ആവശ്യമില്ലാതെ രോഗത്തിൽ നിന്ന് കരകയറുന്നു. കോവിഡ് 19 വരുന്ന ഓരോ 6 പേരിൽ 1 പേർക്ക് ഗുരുതരമായ രോഗം പിടിപെടുകയും ശ്വസിക്കാൻ ബുദ്ധിമുട്ട് ഉണ്ടാകുകയും ചെയ്യുന്നു. പ്രായമായ ആളുകൾ, ഉയർന്ന രക്തസമ്മർദ്ദം, ഹൃദയസംബന്ധമായ പ്രശ്നങ്ങൾ അല്ലെങ്കിൽ പ്രമേഹം പോലുള്ള മെഡിക്കൽ പ്രശ്നങ്ങൾ ഉള്ളവർക്ക് ഗുരുതരമായ രോഗം വരാനുള്ള സാധ്യത കൂടുതലാണ്. പനി, ചുമ, ശ്വസിക്കാൻ ബുദ്ധിമുട്ടുള്ളവർ വൈദ്യസഹായം തേടണം.</t>
+  </si>
+  <si>
+    <t>കൊറോണ വൈറസ് എങ്ങനെ പടരുന്നു?</t>
+  </si>
+  <si>
+    <t>വൈറസ് ബാധിച്ച മറ്റുള്ളവരിൽ നിന്ന് ആളുകൾക്ക് കോവിഡ് 19 പിടിക്കാൻ കഴിയും. മൂക്കിൽ നിന്നോ വായിൽ നിന്നോ ഉള്ള ചെറിയ തുള്ളികളിലൂടെ ഈ രോഗം വ്യക്തിയിൽ നിന്ന് മറ്റൊരാളിലേക്ക് പടരുന്നു, ഇത് കോവിഡ് 19 ചുമ അല്ലെങ്കിൽ ശ്വാസോച്ഛ്വാസം ഉള്ള ഒരാൾക്ക് പടരുന്നു. ഈ തുള്ളികൾ വ്യക്തിക്ക് ചുറ്റുമുള്ള വസ്തുക്കളിലും ഉപരിതലത്തിലും ഇറങ്ങുന്നു. മറ്റ് ആളുകൾ ഈ വസ്തുക്കളെയോ ഉപരിതലത്തെയോ സ്പർശിച്ചുകൊണ്ട് കണ്ണുകൾ, മൂക്ക് അല്ലെങ്കിൽ വായിൽ സ്പർശിച്ചുകൊണ്ട് കോവിഡ് 19 പിടിക്കുന്നു. കോവിഡ് 19 ഉള്ള ഒരു വ്യക്തിയിൽ നിന്ന് തുള്ളിമരുന്ന് ശ്വസിച്ചാൽ ആളുകൾക്ക് കോവിഡ് 19 പിടിക്കാം. അതുകൊണ്ടാണ് രോഗിയായ ഒരാളിൽ നിന്ന് 1 മീറ്ററോ 3 അടിയിലധികം അകലെ നിൽക്കേണ്ടത് പ്രധാനമാണ്.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> കൊറോണ വൈറസിൽ നിന്ന് ഞാൻ എങ്ങനെ സ്വയം പരിരക്ഷിക്കും?</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;പതിവായി ശരിയായി സോപ്പും വെള്ളവും ഉപയോഗിച്ച് കൈ കഴുകുക, അല്ലെങ്കിൽ മദ്യം അടിസ്ഥാനമാക്കിയുള്ള ഹാൻഡ് സാനിറ്റൈസർ ഉപയോഗിച്ച് വൃത്തിയാക്കുക നിങ്ങളുടെ കൈകളിലുള്ള വൈറസുകളെ കൊല്ലുന്നു.&lt;/li&gt;&lt;li&gt;നിങ്ങൾക്കും ചുമയോ തുമ്മലോ ഉള്ള ഏതൊരാളും തമ്മിൽ കുറഞ്ഞത് 1 മീറ്റർ അല്ലെങ്കിൽ 3 അടി ദൂരം നിലനിർത്തുക. ആരെങ്കിലും ചുമയോ തുമ്മുകയോ ചെയ്യുമ്പോൾ മൂക്കിൽ നിന്നോ വായിൽ നിന്നോ ചെറിയ ദ്രാവക തുള്ളികൾ തളിക്കുന്നു, അതിൽ വൈറസ് അടങ്ങിയിരിക്കാം. നിങ്ങൾ വളരെ അടുത്താണെങ്കിൽ, ചുമ ചെയ്യുന്ന വ്യക്തിക്ക് രോഗമുണ്ടെങ്കിൽ കോവിഡ് 19 വൈറസ് ഉൾപ്പെടെയുള്ള തുള്ളികളിൽ ശ്വസിക്കാം.&lt;/li&gt;&lt;li&gt;കണ്ണുകൾ, മൂക്ക്, വായ എന്നിവ തൊടുന്നത് ഒഴിവാക്കുക. &lt;/li&gt;&lt;li&gt;ചുമയോ തുമ്മലോ വരുമ്പോൾ വളഞ്ഞ കൈമുട്ട് അല്ലെങ്കിൽ ടിഷ്യു ഉപയോഗിച്ച് വായും മൂക്കും മൂടുക. ഉപയോഗിച്ച ടിഷ്യു ഉടനടി നീക്കം ചെയ്യുക.&lt;/li&gt;&lt;li&gt;നിങ്ങൾക്ക് അസുഖം തോന്നുന്നുവെങ്കിൽ വീട്ടിൽ തന്നെ തുടരുക. നിങ്ങൾക്ക് പനിയും ചുമയും ശ്വസിക്കാൻ ബുദ്ധിമുട്ടും ഉണ്ടെങ്കിൽ വൈദ്യസഹായം തേടുകയും മുൻകൂട്ടി വിളിക്കുകയും ചെയ്യുക. &lt;/li&gt;&lt;li&gt;നിങ്ങളുടെ പ്രാദേശിക ആരോഗ്യ അതോറിറ്റിയുടെ നിർദ്ദേശങ്ങൾ പാലിക്കുക&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>എനിക്ക് കൊറാണാവൈറസ് ലക്ഷണങ്ങളുണ്ടെങ്കിൽ എന്തുചെയ്യണം?</t>
+  </si>
+  <si>
+    <t>1075 (ടോൾ ഫ്രീ) അല്ലെങ്കിൽ + 91-11-23978046 എന്ന നമ്പറിലേക്കുള്ള ഫോൺ കോൾ ചെയ്യുക.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ಕರೋನವೈರಸ್ಗಳು ವೈರಸ್ಗಳ ದೊಡ್ಡ ಕುಟುಂಬವಾಗಿದ್ದು ಅದು ಪ್ರಾಣಿಗಳಲ್ಲಿ ಅಥವಾ ಮಾನವರಲ್ಲಿ ಅನಾರೋಗ್ಯಕ್ಕೆ ಕಾರಣವಾಗಬಹುದು. </t>
+  </si>
+  <si>
+    <t>ನನ್ನನ್ನು ರಕ್ಷಿಸಿಕೊಳ್ಳಲು ಮತ್ತು ರೋಗ ಹರಡುವುದನ್ನು ತಡೆಯಲು ನಾನು ಏನು ಮಾಡಬಹುದು?</t>
+  </si>
+  <si>
+    <t>ಕರೋನಾ ವೈರಸ್ ಎಂದರೇನು?</t>
+  </si>
+  <si>
+    <t>Covid 19 ಎಂದರೇನು?</t>
+  </si>
+  <si>
+    <t>Covid 19 ನ ಲಕ್ಷಣಗಳು ಯಾವುವು?</t>
+  </si>
+  <si>
+    <t>Covid 19 ಹೇಗೆ ಹರಡುತ್ತದೆ?</t>
+  </si>
+  <si>
+    <t>Covid 19 ಎಂಬುದು ಇತ್ತೀಚೆಗೆ ಪತ್ತೆಯಾದ ಕೊರೊನಾವೈರಸ್‌ನಿಂದ ಉಂಟಾಗುವ ಸಾಂಕ್ರಾಮಿಕ ಕಾಯಿಲೆಯಾಗಿದೆ. ಚೀನಾದ ವುಹಾನ್‌ನಲ್ಲಿ 2019 ರ ಡಿಸೆಂಬರ್‌ನಲ್ಲಿ ಏಕಾಏಕಿ ಪ್ರಾರಂಭವಾಗುವ ಮೊದಲು ಈ ಹೊಸ ವೈರಸ್ ಮತ್ತು ರೋಗ ತಿಳಿದಿಲ್ಲ.</t>
+  </si>
+  <si>
+    <t>Covid 19 ನ ಸಾಮಾನ್ಯ ಲಕ್ಷಣಗಳು ಜ್ವರ, ದಣಿವು ಮತ್ತು ಒಣ ಕೆಮ್ಮು. ಕೆಲವು ರೋಗಿಗಳಿಗೆ ನೋವು ಮತ್ತು ನೋವು, ಮೂಗಿನ ದಟ್ಟಣೆ, ಸ್ರವಿಸುವ ಮೂಗು, ನೋಯುತ್ತಿರುವ ಗಂಟಲು ಅಥವಾ ಅತಿಸಾರ ಇರಬಹುದು. ಈ ಲಕ್ಷಣಗಳು ಸಾಮಾನ್ಯವಾಗಿ ಸೌಮ್ಯವಾಗಿರುತ್ತವೆ ಮತ್ತು ಕ್ರಮೇಣ ಪ್ರಾರಂಭವಾಗುತ್ತವೆ. ಕೆಲವು ಜನರು ಸೋಂಕಿಗೆ ಒಳಗಾಗುತ್ತಾರೆ ಆದರೆ ಯಾವುದೇ ರೋಗಲಕ್ಷಣಗಳನ್ನು ಬೆಳೆಸಿಕೊಳ್ಳಬೇಡಿ ಮತ್ತು ಅನಾರೋಗ್ಯ ಅನುಭವಿಸುವುದಿಲ್ಲ. ಹೆಚ್ಚಿನ ಜನರು (ಸುಮಾರು 80%) ವಿಶೇಷ ಚಿಕಿತ್ಸೆಯ ಅಗತ್ಯವಿಲ್ಲದೆ ರೋಗದಿಂದ ಚೇತರಿಸಿಕೊಳ್ಳುತ್ತಾರೆ. Covid 19 ಪಡೆಯುವ ಪ್ರತಿ 6 ಜನರಲ್ಲಿ ಒಬ್ಬರು ತೀವ್ರವಾಗಿ ಅನಾರೋಗ್ಯಕ್ಕೆ ಒಳಗಾಗುತ್ತಾರೆ ಮತ್ತು ಉಸಿರಾಟದ ತೊಂದರೆ ಉಂಟಾಗುತ್ತದೆ. ವಯಸ್ಸಾದ ಜನರು, ಮತ್ತು ಅಧಿಕ ರಕ್ತದೊತ್ತಡ, ಹೃದಯ ಸಮಸ್ಯೆಗಳು ಅಥವಾ ಮಧುಮೇಹದಂತಹ ವೈದ್ಯಕೀಯ ಸಮಸ್ಯೆಗಳಿರುವವರು ಗಂಭೀರ ಕಾಯಿಲೆಗೆ ಒಳಗಾಗುವ ಸಾಧ್ಯತೆ ಹೆಚ್ಚು. ಜ್ವರ, ಕೆಮ್ಮು ಮತ್ತು ಉಸಿರಾಟದ ತೊಂದರೆ ಇರುವವರು ವೈದ್ಯಕೀಯ ಚಿಕಿತ್ಸೆ ಪಡೆಯಬೇಕು.</t>
+  </si>
+  <si>
+    <t>ಜನರು ವೈರಸ್ ಹೊಂದಿರುವ ಇತರರಿಂದ Covid 19 ಅನ್ನು ಹಿಡಿಯಬಹುದು. ಮೂಗು ಅಥವಾ ಬಾಯಿಯಿಂದ ಸಣ್ಣ ಹನಿಗಳ ಮೂಲಕ ಈ ರೋಗವು ವ್ಯಕ್ತಿಯಿಂದ ವ್ಯಕ್ತಿಗೆ ಹರಡಬಹುದು, ಇದು Covid 19 ಕೆಮ್ಮು ಅಥವಾ ಉಸಿರಾಡುವಾಗ ಹರಡುತ್ತದೆ. ಈ ಹನಿಗಳು ವ್ಯಕ್ತಿಯ ಸುತ್ತಲಿನ ವಸ್ತುಗಳು ಮತ್ತು ಮೇಲ್ಮೈಗಳಲ್ಲಿ ಇಳಿಯುತ್ತವೆ. ಇತರ ಜನರು ಈ ವಸ್ತುಗಳು ಅಥವಾ ಮೇಲ್ಮೈಗಳನ್ನು ಸ್ಪರ್ಶಿಸುವ ಮೂಲಕ Covid 19 ಅನ್ನು ಹಿಡಿಯುತ್ತಾರೆ, ನಂತರ ಅವರ ಕಣ್ಣು, ಮೂಗು ಅಥವಾ ಬಾಯಿಯನ್ನು ಸ್ಪರ್ಶಿಸುತ್ತಾರೆ. Covid 19 ಹೊಂದಿರುವ ವ್ಯಕ್ತಿಯಿಂದ ಹನಿಗಳನ್ನು ಉಸಿರಾಡಿದರೆ ಜನರು Covid 19 ಅನ್ನು ಹಿಡಿಯಬಹುದು ಅಥವಾ ಅವರು ಕೆಮ್ಮುತ್ತಾರೆ ಅಥವಾ ಹನಿಗಳನ್ನು ಬಿಡುತ್ತಾರೆ. ಇದಕ್ಕಾಗಿಯೇ ಅನಾರೋಗ್ಯದಿಂದ ಬಳಲುತ್ತಿರುವ ವ್ಯಕ್ತಿಯಿಂದ 1 ಮೀಟರ್ (3 ಅಡಿ) ಗಿಂತ ಹೆಚ್ಚು ದೂರವಿರುವುದು ಮುಖ್ಯವಾಗಿದೆ.</t>
+  </si>
+  <si>
+    <t>ನಿಯಮಿತವಾಗಿ ಮತ್ತು ಸಂಪೂರ್ಣವಾಗಿ ನಿಮ್ಮ ಕೈಗಳನ್ನು ಆಲ್ಕೋಹಾಲ್ ಆಧಾರಿತ ಹ್ಯಾಂಡ್ ರಬ್ನಿಂದ ಸ್ವಚ್ clean ಗೊಳಿಸಿ ಅಥವಾ ಸೋಪ್ ಮತ್ತು ನೀರಿನಿಂದ ತೊಳೆಯಿರಿ.
+ಏಕೆ? ನಿಮ್ಮ ಕೈಗಳನ್ನು ಸೋಪ್ ಮತ್ತು ನೀರಿನಿಂದ ತೊಳೆಯುವುದು ಅಥವಾ ಆಲ್ಕೋಹಾಲ್ ಆಧಾರಿತ ಹ್ಯಾಂಡ್ ರಬ್ ಬಳಸುವುದರಿಂದ ನಿಮ್ಮ ಕೈಯಲ್ಲಿರುವ ವೈರಸ್‌ಗಳನ್ನು ಕೊಲ್ಲುತ್ತದೆ.
+ನಿಮ್ಮ ಮತ್ತು ಕೆಮ್ಮು ಅಥವಾ ಸೀನುವವರ ನಡುವೆ ಕನಿಷ್ಠ 1 ಮೀಟರ್ (3 ಅಡಿ) ಅಂತರವನ್ನು ಕಾಪಾಡಿಕೊಳ್ಳಿ.
+ಏಕೆ? ಯಾರಾದರೂ ಕೆಮ್ಮಿದಾಗ ಅಥವಾ ಸೀನುವಾಗ ಅವರು ಮೂಗು ಅಥವಾ ಬಾಯಿಯಿಂದ ಸಣ್ಣ ದ್ರವ ಹನಿಗಳನ್ನು ಸಿಂಪಡಿಸುತ್ತಾರೆ, ಅದು ವೈರಸ್ ಅನ್ನು ಹೊಂದಿರಬಹುದು. ನೀವು ತುಂಬಾ ಹತ್ತಿರದಲ್ಲಿದ್ದರೆ, ಕೆಮ್ಮುವ ವ್ಯಕ್ತಿಗೆ ಕಾಯಿಲೆ ಇದ್ದರೆ ನೀವು Covid 19 ವೈರಸ್ ಸೇರಿದಂತೆ ಹನಿಗಳಲ್ಲಿ ಉಸಿರಾಡಬಹುದು.
+ಕಣ್ಣು, ಮೂಗು ಮತ್ತು ಬಾಯಿಯನ್ನು ಸ್ಪರ್ಶಿಸುವುದನ್ನು ತಪ್ಪಿಸಿ.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -178,6 +244,13 @@
       <color rgb="FF1D1C1D"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -200,12 +273,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -721,7 +800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399ED04B-D5D3-434D-BF90-AB19D926B9A6}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -782,4 +861,138 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8746C265-AC5B-5049-8883-E4DC928B4ADB}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="97" customWidth="1"/>
+    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FEDA16-C195-624F-8AF1-952CB87CBD25}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.33203125" customWidth="1"/>
+    <col min="2" max="2" width="101.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="119" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added bengali, modify about page
</commit_message>
<xml_diff>
--- a/questions/questions.xlsx
+++ b/questions/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samboyadvance/corona_faq/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8A2B30C-3A28-354A-B40E-F5B60F05CA0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2801750-85E6-834A-9EC1-189364EED10D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" activeTab="4" xr2:uid="{A2092434-8E9F-7046-A332-FF9F1643DB7C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" activeTab="6" xr2:uid="{A2092434-8E9F-7046-A332-FF9F1643DB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Marathi" sheetId="4" r:id="rId4"/>
     <sheet name="Malayalam" sheetId="5" r:id="rId5"/>
     <sheet name="Kannada" sheetId="6" r:id="rId6"/>
+    <sheet name="Bengali" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="74">
   <si>
     <t>question</t>
   </si>
@@ -220,11 +221,47 @@
     <t>ಜನರು ವೈರಸ್ ಹೊಂದಿರುವ ಇತರರಿಂದ Covid 19 ಅನ್ನು ಹಿಡಿಯಬಹುದು. ಮೂಗು ಅಥವಾ ಬಾಯಿಯಿಂದ ಸಣ್ಣ ಹನಿಗಳ ಮೂಲಕ ಈ ರೋಗವು ವ್ಯಕ್ತಿಯಿಂದ ವ್ಯಕ್ತಿಗೆ ಹರಡಬಹುದು, ಇದು Covid 19 ಕೆಮ್ಮು ಅಥವಾ ಉಸಿರಾಡುವಾಗ ಹರಡುತ್ತದೆ. ಈ ಹನಿಗಳು ವ್ಯಕ್ತಿಯ ಸುತ್ತಲಿನ ವಸ್ತುಗಳು ಮತ್ತು ಮೇಲ್ಮೈಗಳಲ್ಲಿ ಇಳಿಯುತ್ತವೆ. ಇತರ ಜನರು ಈ ವಸ್ತುಗಳು ಅಥವಾ ಮೇಲ್ಮೈಗಳನ್ನು ಸ್ಪರ್ಶಿಸುವ ಮೂಲಕ Covid 19 ಅನ್ನು ಹಿಡಿಯುತ್ತಾರೆ, ನಂತರ ಅವರ ಕಣ್ಣು, ಮೂಗು ಅಥವಾ ಬಾಯಿಯನ್ನು ಸ್ಪರ್ಶಿಸುತ್ತಾರೆ. Covid 19 ಹೊಂದಿರುವ ವ್ಯಕ್ತಿಯಿಂದ ಹನಿಗಳನ್ನು ಉಸಿರಾಡಿದರೆ ಜನರು Covid 19 ಅನ್ನು ಹಿಡಿಯಬಹುದು ಅಥವಾ ಅವರು ಕೆಮ್ಮುತ್ತಾರೆ ಅಥವಾ ಹನಿಗಳನ್ನು ಬಿಡುತ್ತಾರೆ. ಇದಕ್ಕಾಗಿಯೇ ಅನಾರೋಗ್ಯದಿಂದ ಬಳಲುತ್ತಿರುವ ವ್ಯಕ್ತಿಯಿಂದ 1 ಮೀಟರ್ (3 ಅಡಿ) ಗಿಂತ ಹೆಚ್ಚು ದೂರವಿರುವುದು ಮುಖ್ಯವಾಗಿದೆ.</t>
   </si>
   <si>
-    <t>ನಿಯಮಿತವಾಗಿ ಮತ್ತು ಸಂಪೂರ್ಣವಾಗಿ ನಿಮ್ಮ ಕೈಗಳನ್ನು ಆಲ್ಕೋಹಾಲ್ ಆಧಾರಿತ ಹ್ಯಾಂಡ್ ರಬ್ನಿಂದ ಸ್ವಚ್ clean ಗೊಳಿಸಿ ಅಥವಾ ಸೋಪ್ ಮತ್ತು ನೀರಿನಿಂದ ತೊಳೆಯಿರಿ.
-ಏಕೆ? ನಿಮ್ಮ ಕೈಗಳನ್ನು ಸೋಪ್ ಮತ್ತು ನೀರಿನಿಂದ ತೊಳೆಯುವುದು ಅಥವಾ ಆಲ್ಕೋಹಾಲ್ ಆಧಾರಿತ ಹ್ಯಾಂಡ್ ರಬ್ ಬಳಸುವುದರಿಂದ ನಿಮ್ಮ ಕೈಯಲ್ಲಿರುವ ವೈರಸ್‌ಗಳನ್ನು ಕೊಲ್ಲುತ್ತದೆ.
-ನಿಮ್ಮ ಮತ್ತು ಕೆಮ್ಮು ಅಥವಾ ಸೀನುವವರ ನಡುವೆ ಕನಿಷ್ಠ 1 ಮೀಟರ್ (3 ಅಡಿ) ಅಂತರವನ್ನು ಕಾಪಾಡಿಕೊಳ್ಳಿ.
-ಏಕೆ? ಯಾರಾದರೂ ಕೆಮ್ಮಿದಾಗ ಅಥವಾ ಸೀನುವಾಗ ಅವರು ಮೂಗು ಅಥವಾ ಬಾಯಿಯಿಂದ ಸಣ್ಣ ದ್ರವ ಹನಿಗಳನ್ನು ಸಿಂಪಡಿಸುತ್ತಾರೆ, ಅದು ವೈರಸ್ ಅನ್ನು ಹೊಂದಿರಬಹುದು. ನೀವು ತುಂಬಾ ಹತ್ತಿರದಲ್ಲಿದ್ದರೆ, ಕೆಮ್ಮುವ ವ್ಯಕ್ತಿಗೆ ಕಾಯಿಲೆ ಇದ್ದರೆ ನೀವು Covid 19 ವೈರಸ್ ಸೇರಿದಂತೆ ಹನಿಗಳಲ್ಲಿ ಉಸಿರಾಡಬಹುದು.
-ಕಣ್ಣು, ಮೂಗು ಮತ್ತು ಬಾಯಿಯನ್ನು ಸ್ಪರ್ಶಿಸುವುದನ್ನು ತಪ್ಪಿಸಿ.</t>
+    <t>&lt;ul&gt;&lt;li&gt;ನಿಯಮಿತವಾಗಿ ಮತ್ತು ಸಂಪೂರ್ಣವಾಗಿ ನಿಮ್ಮ ಕೈಗಳನ್ನು ಆಲ್ಕೋಹಾಲ್ ಆಧಾರಿತ ಹ್ಯಾಂಡ್ ರಬ್ನಿಂದ ಸ್ವಚ್ clean ಗೊಳಿಸಿ ಅಥವಾ ಸೋಪ್ ಮತ್ತು ನೀರಿನಿಂದ ತೊಳೆಯಿರಿ.&lt;/li&gt;
+&lt;li&gt;ಏಕೆ? ನಿಮ್ಮ ಕೈಗಳನ್ನು ಸೋಪ್ ಮತ್ತು ನೀರಿನಿಂದ ತೊಳೆಯುವುದು ಅಥವಾ ಆಲ್ಕೋಹಾಲ್ ಆಧಾರಿತ ಹ್ಯಾಂಡ್ ರಬ್ ಬಳಸುವುದರಿಂದ ನಿಮ್ಮ ಕೈಯಲ್ಲಿರುವ ವೈರಸ್‌ಗಳನ್ನು ಕೊಲ್ಲುತ್ತದೆ.&lt;/li&gt;
+&lt;li&gt;ನಿಮ್ಮ ಮತ್ತು ಕೆಮ್ಮು ಅಥವಾ ಸೀನುವವರ ನಡುವೆ ಕನಿಷ್ಠ 1 ಮೀಟರ್ (3 ಅಡಿ) ಅಂತರವನ್ನು ಕಾಪಾಡಿಕೊಳ್ಳಿ.&lt;/li&gt;
+&lt;li&gt;ಏಕೆ? ಯಾರಾದರೂ ಕೆಮ್ಮಿದಾಗ ಅಥವಾ ಸೀನುವಾಗ ಅವರು ಮೂಗು ಅಥವಾ ಬಾಯಿಯಿಂದ ಸಣ್ಣ ದ್ರವ ಹನಿಗಳನ್ನು ಸಿಂಪಡಿಸುತ್ತಾರೆ, ಅದು ವೈರಸ್ ಅನ್ನು ಹೊಂದಿರಬಹುದು. ನೀವು ತುಂಬಾ ಹತ್ತಿರದಲ್ಲಿದ್ದರೆ, ಕೆಮ್ಮುವ ವ್ಯಕ್ತಿಗೆ ಕಾಯಿಲೆ ಇದ್ದರೆ ನೀವು Covid 19 ವೈರಸ್ ಸೇರಿದಂತೆ ಹನಿಗಳಲ್ಲಿ ಉಸಿರಾಡಬಹುದು.&lt;/li&gt;
+&lt;li&gt;ಕಣ್ಣು, ಮೂಗು ಮತ್ತು ಬಾಯಿಯನ್ನು ಸ್ಪರ್ಶಿಸುವುದನ್ನು ತಪ್ಪಿಸಿ.&lt;/li&gt;&lt;li&gt;ನೀವು ಕೆಮ್ಮುವಾಗ ಅಥವಾ ಸೀನುವಾಗ ನಿಮ್ಮ ಬಗ್ಗಿದ  ಮೊಣಕೈ ಅಥವಾ ಟಿಶ್ಯೂ ದಿಂದ  ನಿಮ್ಮ ಬಾಯಿ ಮತ್ತು ಮೂಗನ್ನು ಮುಚ್ಚಿ. ನಂತರ ಬಳಸಿ ಟಿಸ್ಸುದನ್ನು  ತಕ್ಷಣ ವಿಲೇವಾರಿ ಮಾಡಿ.&lt;/li&gt;&lt;li&gt;ನಿಮಗೆ ಅನಾರೋಗ್ಯ ಅನಿಸಿದರೆ ಮನೆಯಲ್ಲೇ ಇರಿ. ನಿಮಗೆ ಜ್ವರ, ಕೆಮ್ಮು ಮತ್ತು ಉಸಿರಾಟದ ತೊಂದರೆ ಇದ್ದರೆ, ವೈದ್ಯಕೀಯ ಚಿಕಿತ್ಸೆ ಪಡೆಯಿರಿ ಮತ್ತು ಮುಂಚಿತವಾಗಿ ಕರೆ ಮಾಡಿ.&lt;/li&gt;&lt;li&gt;ನಿಮ್ಮ ಸ್ಥಳೀಯ ಆರೋಗ್ಯ ಪ್ರಾಧಿಕಾರದ ನಿರ್ದೇಶನಗಳನ್ನು ಅನುಸರಿಸಿ&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>ನಾನು ಕರೋನವೈರಸ್ ಲಕ್ಷಣಗಳನ್ನು ಹೊಂದಿದ್ದರೆ ಏನು ಮಾಡಬೇಕು?</t>
+  </si>
+  <si>
+    <t>1075 (ಟೋಲ್ ಫ್ರೀ) ಅಥವಾ + 91-11-23978046 ಗೆ ಫೋನ್ ಕರೆ ಮಾಡಿ</t>
+  </si>
+  <si>
+    <t>করোনা ভাইরাসের লক্ষণগুলি কি কি?</t>
+  </si>
+  <si>
+    <t>করোনা ভাইরাস কীভাবে ছড়িয়ে পড়ে?</t>
+  </si>
+  <si>
+    <t>আমি নিজেকে কীভাবে করোনা ভাইরাস থেকে রক্ষা করব?</t>
+  </si>
+  <si>
+    <t>আপনার  করোনা ভাইরাসের  লক্ষণ থাকলে কী করবেন?</t>
+  </si>
+  <si>
+    <t>১০৭৫ (টোল ফ্রি) ও +৯১-১১-২৩৯৭৮০৪৬ নম্বর এ কল করুন</t>
+  </si>
+  <si>
+    <t>কোভিড ১৯ এর সবচেয়ে সাধারণ লক্ষণগুলি হল জ্বর, ক্লান্তি এবং শুকনো কাশি। কিছু রোগীর শরীরে ব্যথা, অবরুদ্ধ নাক, সর্দি, গলা ব্যথা বা ডায়রিয়া হতে পারে। লক্ষণগুলি সাধারণত হালকা এবং ধীরে ধীরে শুরু হয়। কিছু লোকের ক্ষেত্রে সংক্রামিত হলেও কোনও উপসর্গ বিকাশ করে না এবং অসুস্থ বোধ করে না। প্রায় ৫ জনের মধ্যে ১ জন বিশেষ চিকিত্সার প্রয়োজন ছাড়াই এই রোগ থেকে সেরে উঠেন। কোভিড আক্রান্তের মধ্যে প্রতি ৬ জনের মধ্যে ১ জন গুরুতর অসুস্থ হয়ে পড়ে এবং শ্বাস নিতে অসুবিধা বোধ করে। বয়স্ক ব্যক্তিরা এবং যারা উচ্চ রক্তচাপ, হার্টের সমস্যা বা ডায়াবেটিসের মতো রোগে চিকিত্সাধীন তাদের গুরুতর অসুস্থ হওয়ার সম্ভাবনা বেশি থাকে। জ্বর, কাশি এবং শ্বাস নিতে অসুবিধাজনিত ব্যক্তিদের চিকিত্সার পরামর্শ নেওয়া উচিত।</t>
+  </si>
+  <si>
+    <t>লোকেরা ভাইরাসযুক্ত অন্যদের কাছ থেকে কোভিড ১৯ সংক্রামিত হতে পারে। কোভিড ১৯ সংক্রামিত কোনো ব্যক্তির কাশি বা শ্বাস ছাড়ার সময় নাক বা মুখ থেকে ছোট ফোঁটাগুলির মাধ্যমে এই রোগটি এক ব্যক্তি থেকে অন্য ব্যক্তির কাছে ছড়িয়ে পড়ে। এই ফোঁটাগুলি ব্যক্তিটির চারপাশে বস্তু এবং পৃষ্ঠগুলিতে অবতরণ করে। অন্যান্য ব্যক্তিরা তখন এই জিনিসগুলি বা পৃষ্ঠের স্পর্শ করে, তারপর তাদের চোখ, নাক বা মুখ স্পর্শ করে তখন তারা সংক্রমিত হন। যদি কোনো বেক্তি, কোভিড ১৯ সংক্রামিত কোনো ব্যক্তির কাশি বা শ্বাস ছাড়ার সময়ের ফোঁটাগুলি শ্বাসের মাধ্যমে শরীরের ভিতরে প্রবেশ করান তাহলেও সংক্রমন হতে পারে। এজন্য অসুস্থ ব্যক্তির থেকে ১ মিটার বা ৩ ফুট বেশি দূরে থাকা গুরুত্বপূর্ণ।</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;নিয়মিত এবং সঠিকভাবে সাবান এবং জল দিয়ে আপনার হাত ধুলে, বা অ্যালকোহল ভিত্তিক হাতের স্যানিটাইজার দিয়ে পরিষ্কার করলে আপনার হাতের ভাইরাসগুলি মরে যাবে। &lt;/li&gt; &lt;li&gt;নিজের এবং কাশি বা হাঁচি হয় এমন কারও মধ্যে অন্তত ১ মিটার বা ৩ ফুট দূরত্ব বজায় রাখুন। যখন কেউ কাশি বা হাঁচে তখন তারা তাদের নাক বা মুখ থেকে ছোট তরল ফোঁটা স্প্রে করে যার মধ্যে ভাইরাস থাকতে পারে। যদি আপনি কোনো কোভিড ১৯ সংক্রমিত ব্যক্তির খুব কাছাকাছি থাকেন তাহলে তার কাশির সাথে ভাইরাস আপনার শরীরের ভিতরে প্রবেশ করতে পারে। &lt;/li&gt; &lt;li&gt;চোখ, নাক এবং মুখ স্পর্শ করা এড়িয়ে চলুন।&lt;/li&gt; &lt;li&gt;কাশি বা হাঁচি হলে আপনার বাঁকানো কনুই বা টিস্যু দিয়ে আপনার মুখ এবং নাকটি ঢেকে রাখুন। তারপরে অবিলম্বে ব্যবহৃত টিস্যুগুলি ফেলে দিন। &lt;/li&gt; &lt;li&gt;আপনি অসুস্থ বোধ করলে বাড়িতেই থাকুন। আপনার যদি জ্বর, কাশি এবং শ্বাস নিতে সমস্যা হয় তবে চিকিত্সার পরামর্শ নিন এবং আগে থেকেই কল করুন।&lt;/li&gt; &lt;li&gt;আপনার স্থানীয় স্বাস্থ্য কর্তৃপক্ষের নির্দেশাবলী অনুসরণ করুন।&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>করোনা ভাইরাস বা কোভিড ১৯ কি?</t>
+  </si>
+  <si>
+    <t>করোনা ভাইরাস হল এক ধরণের ভাইরাস যা প্রাণী বা মানুষের সাধারণ সর্দি বা আরও গুরুতর অসুস্থতার কারণ হতে পারে।কোভিড ১৯ হল এক ধরণের করোনা  ভাইরাস যা সম্প্রতি ২০১৯ সালে চিনে পাওয়া গিয়েছিল এবং এটি ভারত সহ বিশ্বের বিভিন্ন জায়গায় ছড়িয়ে পড়েছে।</t>
   </si>
 </sst>
 </file>
@@ -602,7 +639,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -867,7 +904,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8746C265-AC5B-5049-8883-E4DC928B4ADB}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
@@ -932,7 +969,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23FEDA16-C195-624F-8AF1-952CB87CBD25}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -984,12 +1021,86 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="153" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="204" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C24EEF-86B5-5948-B0B7-80DE1B0DD836}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="66.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add telugu, modify about page
</commit_message>
<xml_diff>
--- a/questions/questions.xlsx
+++ b/questions/questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samboyadvance/corona_faq/questions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FF31012-985E-2B48-8209-05AB699B0282}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8786D0-1CA6-1D4C-8B4C-E18C46CAA988}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" activeTab="7" xr2:uid="{A2092434-8E9F-7046-A332-FF9F1643DB7C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="40960" windowHeight="22580" activeTab="8" xr2:uid="{A2092434-8E9F-7046-A332-FF9F1643DB7C}"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="Kannada" sheetId="6" r:id="rId6"/>
     <sheet name="Bengali" sheetId="7" r:id="rId7"/>
     <sheet name="Tamil" sheetId="8" r:id="rId8"/>
+    <sheet name="Telugu" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>question</t>
   </si>
@@ -300,12 +301,42 @@
   <si>
     <t xml:space="preserve">1075 என்ற இலவச அழைப்பு எண்ணையோ  அல்லது +91-11-23978046 என்ற எண்ணையோ  உடனே அழையுங்கள் </t>
   </si>
+  <si>
+    <t> కరోనా వైరస్ / కోవిడ్ 19 అంటే ఏమిటి?</t>
+  </si>
+  <si>
+    <t> కరోనా వైరస్ యొక్క లక్షణాలు ఏమిటి?</t>
+  </si>
+  <si>
+    <t> కరోనా వైరస్ ఎలా వ్యాపిస్తుంది?</t>
+  </si>
+  <si>
+    <t> కరోనా వైరస్ నుండి నన్ను నేను ఎలా రక్షించుకోవాలి?</t>
+  </si>
+  <si>
+    <t>నాకు కరోనా వైరస్ లక్షణాలు ఉంటే ఏమి చేయాలి?</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;సరిగా మరియు క్రమం తప్పకుండా సబ్బు మరియు నీటితో మీ చేతులు కడుక్కోవడం, లేదా ఆల్కహాల్ బేస్డ్ హ్యాండ్ శానిటైజర్ తో శుభ్రం చేసుకోవడం వల్ల మీ చేతుల్లో ఉండే వైరస్లను చంపవచ్చు.&lt;/li&gt;&lt;li&gt;దగ్గు లేదా తుమ్ము ఉన్నవారికి మరియు మీకు మధ్య కనీసం 1 మీటర్ లేదా 3 అడుగుల దూరం ఉండేలా చూసుకోవాలి. ఎవరైనా దగ్గినప్పుడు లేదా తుమ్మినప్పుడు, వారు ముక్కు లేదా నోటి నుండి చిన్న ద్రవ బిందువులను పిచికారీ చేస్తారు, ఇందులో వైరస్ ఉండవచ్చు. మరియు ఆ వ్యక్తికి కోవిడ్ 19 వుండే అవకాశం కూడా ఉండవచ్చు, మీరు వారికి చాలా దగ్గరగా ఉంటే, ఆ బిందువులని శ్వాస ద్వారా తీసుకునే అవకాశం ఉండవచ్చు.&lt;/li&gt;&lt;li&gt;కళ్ళు, ముక్కు మరియు నోరు తాకడం మానుకోవాలి.&lt;/li&gt;&lt;li&gt;మీరు మీరు దగ్గినప్పుడు లేదా తుమ్మినప్పుడు, మీ నోరు మరియు ముక్కును మీ మోచేయి లేదా టిష్యూ పేపర్తో అడ్డుపెట్టుకోండి. ఆ వాడిన టిష్యూ పేపర్ని వెంటనే పారవేయండి.&lt;/li&gt;&lt;li&gt;మీకు అనారోగ్యం అనిపిస్తే ఇంట్లోనే ఉండండి. మీకు జ్వరం, దగ్గు మరియు శ్వాస తీసుకోవడంలో ఇబ్బంది ఉంటే, వైద్య సహాయం తీసుకోండి మరియు ముందుగానే వైద్యులకు కాల్ చేసి వారి సూచనలు తీసుకోండి.&lt;/li&gt;&lt;li&gt;మీ స్థానిక ఆరోగ్య అధికారుల యొక్క సూచనలను అనుసరించండి.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t> 1075 (టోల్ ఫ్రీ) లేదా +91-11-23978046 కు ఫోన్ చేయండి.</t>
+  </si>
+  <si>
+    <t>కరోనావైరస్ అనేది ఒక రకమైన వైరస్, ఇది జంతువులలో లేదా మానవులలో అనారోగ్యానికి కారణమవుతుంది, జలుబు లేదా మరింత తీవ్రమైన అనారోగ్యాలు వంటివి. కోవిడ్ 19 అనేది ఒక రకమైన కరోనావైరస్, ఇది ఇటీవల 2019 లో చైనాలో కనుగొనబడింది మరియు ఇది భారతదేశంతో సహా ప్రపంచంలోని వివిధ ప్రాంతాలకు వ్యాపించింది.</t>
+  </si>
+  <si>
+    <t>కోవిడ్ 19 యొక్క సాధారణ లక్షణాలు జ్వరం, అలసట మరియు పొడి దగ్గు. కొంతమంది రోగులకు శరీర నొప్పి, ముక్కు దిబ్బడ, ముక్కు కారటం, గొంతు నొప్పి లేదా విరేచనాలు ఉండవచ్చు. ఈ లక్షణాలు సాధారణంగా తేలికపాటివి మరియు క్రమంగా ప్రారంభమవుతాయి. కొంతమంది వ్యాధి బారిన పడినను కూడా, ఎటువంటి వ్యాధి లక్షణాలని చూపరు మరియు అనారోగ్యంగా అనిపించరు. 5 మందిలో 1 మందికి ప్రత్యేక చికిత్స అవసరం లేకుండానే వ్యాధి నుండి కోలుకుంటారు. కోవిడ్ 19 వచ్చే ప్రతి 6 మందిలో ఒకరు తీవ్రంగా అనారోగ్యానికి గురవుతారు మరియు శ్వాస తీసుకోవడంలో ఇబ్బంది పడతారు. వృద్ధులు, మరియు అధిక రక్తపోటు, గుండె సమస్యలు లేదా డయాబెటిస్ వంటి వైద్య సమస్యలు ఉన్నవారికి తీవ్రమైన అనారోగ్యం వచ్చే అవకాశం ఉంది. జ్వరం, దగ్గు మరియు శ్వాస తీసుకోవడంలో ఇబ్బంది ఉన్నవారు వైద్య సహాయం తీసుకోవాలి.</t>
+  </si>
+  <si>
+    <t>వైరస్ ఉన్న ఇతరుల నుండి కోవిడ్ 19 ప్రజలకు వ్యాపిస్తుంది. కోవిడ్ 19 వున్న వ్యక్తి తుమ్మినప్పుడు లేదా దగ్గినప్పుడు, ముక్కు లేదా నోటి నుండి వచ్చే చిన్న చిన్న బిందువుల ద్వారా ఈ వ్యాధి ఒక వ్యక్తి నుండి మరొక వ్యక్తికి వ్యాపిస్తుంది. ఈ బిందువులు వ్యక్తి చుట్టూ ఉన్న వస్తువులు మరియు ఉపరితలాలపైన పడతాయి. ఈ వస్తువులను లేదా ఉపరితలాలను తాకి, వారి కళ్ళు, ముక్కు లేదా నోటిని తాకడం ద్వారా కోవిడ్ 19 ఇతర వ్యక్తులకు వ్యాపిస్తుంది. కోవిడ్ 19 ఉన్న వ్యక్తి తుమ్మినప్పుడు లేదా దగ్గినప్పుడు వచ్చే బిందువులని  ఊపిరి ద్వారా పీల్చడం వలన కూడా ప్రజలకు కోవిడ్ 19 వ్యాపిస్తుంది. అందువలన అనారోగ్యంతో ఉన్న వ్యక్తికి 1 మీటర్ లేదా 3 అడుగుల కన్నా ఎక్కువ దూరంగా ఉండటం చాలా ముఖ్యం.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -325,6 +356,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -347,7 +384,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -359,6 +396,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1149,7 +1187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A14D9218-17E6-9741-99AD-FA2E90BDF5F0}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -1209,4 +1247,71 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E08C95DE-EA27-C747-B1E4-A115889DE069}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="104.6640625" customWidth="1"/>
+    <col min="2" max="2" width="68.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>